<commit_message>
jn: dos diccionarios finales
</commit_message>
<xml_diff>
--- a/04_Entregable 2/previo/metadatos y diccionario_17.xlsx
+++ b/04_Entregable 2/previo/metadatos y diccionario_17.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco_F\!!Personal\Mio\1_WCS 2024\wcs\04_Entregable 2\previo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Javi_Angelito\wcs\04_Entregable 2\previo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29726424-D9C4-47EC-89F6-7BAE628EB0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11385" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadatos generales" sheetId="1" r:id="rId1"/>
@@ -29,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -68,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
         <r>
           <rPr>
@@ -85,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="169">
   <si>
     <t>Elemento</t>
   </si>
@@ -540,9 +541,6 @@
   </si>
   <si>
     <t>Geolocalización</t>
-  </si>
-  <si>
-    <t>Evento</t>
   </si>
   <si>
     <t>ESMERALDAS</t>
@@ -623,7 +621,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
@@ -728,7 +726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -755,7 +753,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -767,60 +765,57 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="21" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="21" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -828,71 +823,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1184,7 +1115,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1205,7 +1136,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1252,7 +1183,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1414,7 +1345,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>24</v>
       </c>
@@ -1465,7 +1396,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1483,7 +1414,7 @@
         <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1499,7 +1430,7 @@
         <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1518,7 +1449,7 @@
         <v>71</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1526,7 +1457,7 @@
         <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1534,7 +1465,7 @@
         <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1570,647 +1501,646 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E18" sqref="E18:E21"/>
+      <selection pane="topRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="17"/>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="20" t="s">
+      <c r="D2" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="35"/>
+      <c r="F3" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="35"/>
+      <c r="F5" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="J6" s="17"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="J7" s="17"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="35"/>
+      <c r="F8" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="I10" s="17">
+        <v>0.95684967930316001</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="I11" s="17">
+        <v>-79.630504846571995</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="18">
+        <v>43583</v>
+      </c>
+      <c r="J12" s="17"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="J2" s="20"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="20" t="s">
+      <c r="J13" s="17"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="38"/>
-      <c r="F3" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="G3" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="20" t="s">
+      <c r="D14" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="17">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="J15" s="17"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="17">
+        <v>0.625</v>
+      </c>
+      <c r="J16" s="17"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="17">
+        <v>16.309999999999999</v>
+      </c>
+      <c r="J17" s="17"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I4" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="J4" s="20"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="20" t="s">
+      <c r="D18" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="35"/>
+      <c r="F18" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="J18" s="17"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="38"/>
-      <c r="F5" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I5" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="J5" s="20" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="20" t="s">
+      <c r="D19" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="35"/>
+      <c r="F19" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="J19" s="17"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I6" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="J6" s="20"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="20" t="s">
+      <c r="D20" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="35"/>
+      <c r="F20" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="J20" s="17"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="J7" s="20"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C8" s="20" t="s">
+      <c r="D21" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="35"/>
+      <c r="F21" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="J21" s="17"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="I10" s="20">
-        <v>0.95684967930316001</v>
-      </c>
-      <c r="J10" s="20" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="I11" s="20">
-        <v>-79.630504846571995</v>
-      </c>
-      <c r="J11" s="20" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="I12" s="21">
-        <v>43583</v>
-      </c>
-      <c r="J12" s="20"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="J13" s="20"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="I15" s="20">
-        <v>0.51388888888888895</v>
-      </c>
-      <c r="J15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="I16" s="20">
-        <v>0.625</v>
-      </c>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="D22" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="I17" s="20">
-        <v>16.309999999999999</v>
-      </c>
-      <c r="J17" s="20"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="38"/>
-      <c r="F18" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20" t="s">
+      <c r="G22" s="17"/>
+      <c r="H22" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="J18" s="20"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="J19" s="20"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="20" t="s">
-        <v>134</v>
-      </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="I20" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="J20" s="20"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="I21" s="20" t="s">
+      <c r="I22" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="J21" s="20"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="J22" s="20"/>
+      <c r="J22" s="17"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I23" s="20"/>
+      <c r="I23" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2219,7 +2149,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2246,7 +2176,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
@@ -2255,316 +2185,276 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="18"/>
+    <col min="1" max="16384" width="11.42578125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:21" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="N1" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="O1" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="R1" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="S1" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="U1" s="33" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:21" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="M2" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="O2" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="P2" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="Q2" s="23" t="s">
+      <c r="Q2" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="R2" s="22" t="s">
+      <c r="R2" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="S2" s="22" t="s">
+      <c r="S2" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="T2" s="36" t="s">
+      <c r="T2" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="U2" s="36" t="s">
+      <c r="U2" s="33" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:21" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="24" t="s">
         <v>99</v>
       </c>
-      <c r="L3" s="28" t="s">
+      <c r="L3" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="M3" s="37" t="s">
+      <c r="M3" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="N3" s="29" t="s">
+      <c r="N3" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="O3" s="22" t="s">
+      <c r="O3" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="P3" s="22" t="s">
+      <c r="P3" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="Q3" s="23" t="s">
+      <c r="Q3" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="R3" s="22" t="s">
+      <c r="R3" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="S3" s="22" t="s">
+      <c r="S3" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="T3" s="36" t="s">
+      <c r="T3" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="U3" s="36" t="s">
+      <c r="U3" s="33" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="31"/>
-      <c r="S4" s="31"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
+      <c r="A5" s="28"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="28"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L1:M1">
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text=".,;">
-      <formula>NOT(ISERROR(SEARCH((".,;"),(L1))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1">
-    <cfRule type="expression" dxfId="8" priority="12">
+  <conditionalFormatting sqref="L1:L5">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>ISERROR(L1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:M2">
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text=".,;">
-      <formula>NOT(ISERROR(SEARCH((".,;"),(L2))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L2">
-    <cfRule type="expression" dxfId="6" priority="10">
-      <formula>ISERROR(L2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L3:M3">
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text=".,;">
-      <formula>NOT(ISERROR(SEARCH((".,;"),(L3))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L3">
-    <cfRule type="expression" dxfId="4" priority="8">
-      <formula>ISERROR(L3)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L4:M4">
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text=".,;">
-      <formula>NOT(ISERROR(SEARCH((".,;"),(L4))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L4">
-    <cfRule type="expression" dxfId="2" priority="6">
-      <formula>ISERROR(L4)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L5">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>ISERROR(L5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L5:M5">
+  <conditionalFormatting sqref="L1:M5">
     <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text=".,;">
-      <formula>NOT(ISERROR(SEARCH((".,;"),(L5))))</formula>
+      <formula>NOT(ISERROR(SEARCH((".,;"),(L1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>